<commit_message>
refactor and rename shared_memory_cell_state to local_species_population; add read_one() method expand tests of SsaSubmodel rename ExtendedModel as ExecutableModel & extend & test it fix doc strings
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1460" windowWidth="25600" windowHeight="15540" activeTab="3"/>
+    <workbookView xWindow="1600" yWindow="1460" windowWidth="32360" windowHeight="19120" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -136,12 +136,6 @@
   </si>
   <si>
     <t>Km (M)</t>
-  </si>
-  <si>
-    <t>Vmax * Adk-Protein[c]</t>
-  </si>
-  <si>
-    <t>Vmax * min(ATP[c], CTP[c], GTP[c], UTP[c]) / (Km + min(ATP[c], CTP[c], GTP[c], UTP[c])) * RnaPolymerase-Protein[c]</t>
   </si>
   <si>
     <t>Value</t>
@@ -274,6 +268,15 @@
   </si>
   <si>
     <t>[c]: specie_2 + (2) specie_3 &lt;==&gt; specie_4</t>
+  </si>
+  <si>
+    <t>Vmax * specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vmax * min( specie_2[c], specie_3[c]) / 2 </t>
+  </si>
+  <si>
+    <t>Vmax * min( specie_4[c], specie_5[c])</t>
   </si>
 </sst>
 </file>
@@ -773,7 +776,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="A4:C4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -797,7 +800,7 @@
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -808,7 +811,7 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -899,7 +902,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -957,10 +960,10 @@
     </row>
     <row r="2" spans="1:16380" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -978,10 +981,10 @@
     </row>
     <row r="3" spans="1:16380" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -989,15 +992,17 @@
       <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:16380" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
@@ -1008,14 +1013,16 @@
       <c r="H4" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4">
+        <v>1.4799999999999999E-4</v>
+      </c>
     </row>
     <row r="5" spans="1:16380" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -1026,7 +1033,6 @@
       <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -17402,10 +17408,10 @@
     </row>
     <row r="6" spans="1:16380" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -33792,10 +33798,10 @@
     </row>
     <row r="7" spans="1:16380" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -50197,20 +50203,20 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10.5" style="3" customWidth="1"/>
@@ -50253,83 +50259,83 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="G3" s="6">
-        <v>1247</v>
+        <v>2000</v>
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="26" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="G4" s="6">
-        <v>2.3345582123025931E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="H4" s="6">
         <v>1E-3</v>
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="26" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="G5" s="6">
-        <v>2.3345582123025931E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="H5" s="6">
         <v>1E-3</v>
@@ -50381,10 +50387,10 @@
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -50392,87 +50398,87 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3">
         <v>28800</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="3">
         <v>300</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3">
         <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3">
         <v>0.3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run a test simulation involving 3 SimulationObjects, 2 SkeletonSubmodels and a SpeciesPopSimObject. Implement prefetching of species populations from SpeciesPopSimObjects, & caching of prefetched values. use fully qualified names for classes in MessageTypesRegistry to minimize risk if false matches
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1460" windowWidth="32360" windowHeight="19120" activeTab="3"/>
+    <workbookView xWindow="1600" yWindow="1460" windowWidth="32360" windowHeight="19120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Species!$A$1:$L$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Submodels!$A$1:$C$3</definedName>
   </definedNames>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -898,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XEZ7"/>
   <sheetViews>
-    <sheetView zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="209" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="209" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -50202,11 +50202,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD5"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add biological_type to DynamicCompartment; finish testing almost all of wc_sim/dynamic_components.py; remove constants from tests; enhance testing performance; fix some bad automatic formatting
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31680" yWindow="1100" windowWidth="22660" windowHeight="11180" tabRatio="993" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="-9760" yWindow="24560" windowWidth="22880" windowHeight="11740" tabRatio="993" firstSheet="10" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4687,11 +4687,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4880,7 +4880,7 @@
         <v>91</v>
       </c>
       <c r="D12" s="18">
-        <v>1100</v>
+        <v>100</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>226</v>
@@ -5862,11 +5862,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMR9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8132,7 +8132,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8559,11 +8559,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
remake build_simulation(), test build_simulation(), get_dynamic_compartments()
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-9760" yWindow="24560" windowWidth="22880" windowHeight="11740" tabRatio="993" firstSheet="10" activeTab="16"/>
+    <workbookView xWindow="-7960" yWindow="24340" windowWidth="22020" windowHeight="13260" tabRatio="993" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="281">
   <si>
     <t>!!ObjTables TableType='Schema' ObjTablesVersion='0.0.8'</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>dynamic_flux_balance_analysis</t>
-  </si>
-  <si>
-    <t>For testing</t>
   </si>
   <si>
     <t>submodel_2</t>
@@ -1878,7 +1875,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1889,10 +1886,10 @@
         <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>43</v>
@@ -1936,7 +1933,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1947,10 +1944,10 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>43</v>
@@ -1970,26 +1967,26 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2021,7 @@
   <sheetData>
     <row r="1" spans="1:1027" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:1027" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2035,7 +2032,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="25"/>
@@ -3066,25 +3063,25 @@
         <v>30</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>160</v>
-      </c>
       <c r="I3" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>43</v>
@@ -4117,22 +4114,22 @@
     </row>
     <row r="4" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>161</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>162</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E4" s="18">
         <v>0</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G4" s="18">
         <v>0</v>
@@ -4141,69 +4138,69 @@
         <v>1</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>166</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>167</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E5" s="18">
         <v>1</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>170</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>171</v>
       </c>
       <c r="E6" s="18">
         <v>1</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>173</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="E7" s="18">
         <v>0</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -4243,7 +4240,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -4254,19 +4251,19 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>177</v>
-      </c>
       <c r="E2" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>43</v>
@@ -4286,88 +4283,88 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="F3" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>180</v>
-      </c>
       <c r="G3" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>182</v>
-      </c>
       <c r="G4" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>184</v>
-      </c>
       <c r="G5" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>187</v>
-      </c>
       <c r="G6" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>189</v>
-      </c>
       <c r="G7" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M7" s="6"/>
     </row>
@@ -4399,7 +4396,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="42" x14ac:dyDescent="0.2">
@@ -4410,19 +4407,19 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>191</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>192</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>43</v>
@@ -4442,19 +4439,19 @@
     </row>
     <row r="3" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>42</v>
@@ -4489,7 +4486,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -4500,13 +4497,13 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>43</v>
@@ -4526,22 +4523,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -4576,7 +4573,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -4587,16 +4584,16 @@
         <v>30</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>43</v>
@@ -4616,65 +4613,65 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E3" s="9">
         <v>-3</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>205</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" s="9">
         <v>-4</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>207</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="9">
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4687,7 +4684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -4711,7 +4708,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -4722,16 +4719,16 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>43</v>
@@ -4751,150 +4748,150 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>210</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>211</v>
       </c>
       <c r="D3" s="18">
         <v>0.3</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>213</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>214</v>
       </c>
       <c r="D4" s="18">
         <v>1</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>215</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>216</v>
       </c>
       <c r="D5" s="18">
         <v>1</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D6" s="6">
         <v>2000</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D7" s="6">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D8" s="6">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D9" s="6">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>222</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>223</v>
       </c>
       <c r="D10" s="6">
         <v>1E-3</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="6">
         <v>6.02214075862E+23</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="18">
         <v>100</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="18">
         <v>1000</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -4927,7 +4924,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -4938,10 +4935,10 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>43</v>
@@ -4961,16 +4958,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="18" t="s">
         <v>229</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -4998,16 +4995,16 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H2" s="26"/>
       <c r="I2" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
@@ -5015,11 +5012,11 @@
       <c r="M2" s="26"/>
       <c r="N2" s="26"/>
       <c r="Q2" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R2" s="26"/>
       <c r="S2" s="29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T2" s="26"/>
     </row>
@@ -5031,22 +5028,22 @@
         <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>56</v>
@@ -5055,22 +5052,22 @@
         <v>57</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>242</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>30</v>
@@ -5240,7 +5237,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5251,7 +5248,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>43</v>
@@ -5301,12 +5298,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H2" s="26"/>
     </row>
@@ -5318,16 +5315,16 @@
         <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>30</v>
@@ -5348,10 +5345,10 @@
         <v>53</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5420,7 +5417,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -5431,46 +5428,46 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="L2" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="M2" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="O2" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="P2" s="15" t="s">
         <v>261</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>262</v>
       </c>
       <c r="Q2" s="15" t="s">
         <v>43</v>
@@ -5505,7 +5502,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -5516,28 +5513,28 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>270</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>43</v>
@@ -5570,7 +5567,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -5581,28 +5578,28 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>277</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>278</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>43</v>
@@ -5620,10 +5617,10 @@
         <v>53</v>
       </c>
       <c r="P2" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q2" s="15" t="s">
         <v>247</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -5776,11 +5773,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5837,19 +5834,16 @@
         <v>65</v>
       </c>
       <c r="D3" s="16"/>
-      <c r="G3" s="18" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C4" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -5891,7 +5885,7 @@
   <sheetData>
     <row r="1" spans="1:1032" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:1032" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -5903,14 +5897,14 @@
       <c r="F2" s="46"/>
       <c r="G2" s="46"/>
       <c r="H2" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" s="48"/>
       <c r="J2" s="48"/>
       <c r="K2" s="48"/>
       <c r="L2" s="46"/>
       <c r="M2" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
@@ -6940,46 +6934,46 @@
         <v>30</v>
       </c>
       <c r="C3" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="E3" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="F3" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="G3" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="H3" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="I3" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="49" t="s">
+      <c r="J3" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="49" t="s">
+      <c r="K3" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="49" t="s">
+      <c r="L3" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="L3" s="49" t="s">
-        <v>81</v>
-      </c>
       <c r="M3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="O3" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="P3" s="42" t="s">
         <v>79</v>
-      </c>
-      <c r="P3" s="42" t="s">
-        <v>80</v>
       </c>
       <c r="Q3" s="42" t="s">
         <v>43</v>
@@ -8010,28 +8004,28 @@
     </row>
     <row r="4" spans="1:1032" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="C4" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="D4" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="E4" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="F4" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="G4" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="H4" s="50" t="s">
         <v>88</v>
-      </c>
-      <c r="H4" s="50" t="s">
-        <v>89</v>
       </c>
       <c r="I4" s="51">
         <v>4.58E-17</v>
@@ -8040,13 +8034,13 @@
         <v>4.5800000000000003E-18</v>
       </c>
       <c r="K4" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="L4" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="50" t="s">
-        <v>91</v>
-      </c>
       <c r="M4" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N4" s="18">
         <v>7.75</v>
@@ -8055,34 +8049,34 @@
         <v>0.77500000000000002</v>
       </c>
       <c r="P4" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="T4" s="18" t="s">
         <v>92</v>
-      </c>
-      <c r="T4" s="18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1032" s="45" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="53" t="s">
-        <v>95</v>
-      </c>
       <c r="D5" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="53" t="s">
         <v>85</v>
-      </c>
-      <c r="E5" s="53" t="s">
-        <v>86</v>
       </c>
       <c r="F5" s="53"/>
       <c r="G5" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>88</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>89</v>
       </c>
       <c r="I5" s="55">
         <v>9.9999999999999998E-13</v>
@@ -8091,13 +8085,13 @@
         <v>1E-13</v>
       </c>
       <c r="K5" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M5" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N5" s="44">
         <v>7.75</v>
@@ -8106,10 +8100,10 @@
         <v>0.77500000000000002</v>
       </c>
       <c r="P5" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T5" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:1032" ht="14" x14ac:dyDescent="0.15"/>
@@ -8153,12 +8147,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C2" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -8174,25 +8168,25 @@
         <v>30</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>105</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>106</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>43</v>
@@ -8212,10 +8206,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>107</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>108</v>
       </c>
       <c r="G4" s="18">
         <v>1</v>
@@ -8224,16 +8218,16 @@
         <v>0</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>110</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>111</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="18">
@@ -8243,16 +8237,16 @@
         <v>0</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>112</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>113</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="18">
@@ -8262,16 +8256,16 @@
         <v>0</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>114</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>115</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="18">
@@ -8281,16 +8275,16 @@
         <v>0</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>117</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="18">
@@ -8300,34 +8294,34 @@
         <v>0</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>118</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>119</v>
       </c>
       <c r="F9" s="13"/>
       <c r="H9" s="18">
         <v>0</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G10" s="18">
         <v>18.0152</v>
@@ -8336,7 +8330,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -8370,7 +8364,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -8381,13 +8375,13 @@
         <v>30</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>124</v>
-      </c>
       <c r="E2" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>43</v>
@@ -8407,142 +8401,142 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>125</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -8583,7 +8577,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -8600,19 +8594,19 @@
         <v>30</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="F2" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="G2" s="37" t="s">
         <v>79</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>80</v>
       </c>
       <c r="H2" s="30" t="s">
         <v>43</v>
@@ -8632,14 +8626,14 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="35">
         <v>1.4799999999999999E-4</v>
@@ -8648,19 +8642,19 @@
         <v>7.4000000000000003E-6</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="35">
         <v>2.0000000000000001E-4</v>
@@ -8669,121 +8663,121 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="35">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="F5" s="40"/>
       <c r="G5" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" s="35">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="35">
         <v>1E-3</v>
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="34"/>
       <c r="C8" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="35">
         <v>2E-3</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="35">
         <v>1</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="35">
         <v>1</v>
       </c>
       <c r="F10" s="40"/>
       <c r="G10" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add biological_type to compartments made by MakeModel; update TestModelUtilities; fix long line formatting
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-7960" yWindow="24340" windowWidth="22020" windowHeight="13260" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="-11020" yWindow="24340" windowWidth="22020" windowHeight="13260" tabRatio="993" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -2003,7 +2003,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4470,7 +4470,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4555,7 +4555,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5773,11 +5773,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5860,7 +5860,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8126,7 +8126,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:G10"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8347,7 +8347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -8557,7 +8557,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add DynamicModel methods for cell_volume, cell_accounted_mass, & cell_accounted_volume; test them using additional worksheets in test_model.xlsx that calculate expected values
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-11020" yWindow="24340" windowWidth="22020" windowHeight="13260" tabRatio="993" activeTab="7"/>
+    <workbookView xWindow="-22360" yWindow="10460" windowWidth="22360" windowHeight="11140" tabRatio="993" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="9560" windowWidth="33180" windowHeight="12040" tabRatio="500" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -21,49 +22,50 @@
     <sheet name="!!Species types" sheetId="7" r:id="rId7"/>
     <sheet name="!!Species" sheetId="8" r:id="rId8"/>
     <sheet name="!!Initial species concentration" sheetId="9" r:id="rId9"/>
-    <sheet name="!!Observables" sheetId="10" r:id="rId10"/>
-    <sheet name="!!Functions" sheetId="11" r:id="rId11"/>
-    <sheet name="!!Reactions" sheetId="12" r:id="rId12"/>
-    <sheet name="!!Rate laws" sheetId="13" r:id="rId13"/>
-    <sheet name="!!dFBA objectives" sheetId="14" r:id="rId14"/>
-    <sheet name="!!dFBA objective reactions" sheetId="15" r:id="rId15"/>
-    <sheet name="!!dFBA objective species" sheetId="16" r:id="rId16"/>
-    <sheet name="!!Parameters" sheetId="17" r:id="rId17"/>
-    <sheet name="!!Stop conditions" sheetId="18" r:id="rId18"/>
-    <sheet name="!!Observations" sheetId="19" r:id="rId19"/>
-    <sheet name="!!Observation sets" sheetId="20" r:id="rId20"/>
-    <sheet name="!!Conclusions" sheetId="21" r:id="rId21"/>
-    <sheet name="!!References" sheetId="22" r:id="rId22"/>
-    <sheet name="!!Authors" sheetId="23" r:id="rId23"/>
-    <sheet name="!!Changes" sheetId="24" r:id="rId24"/>
+    <sheet name="!!Expected initial values" sheetId="26" r:id="rId10"/>
+    <sheet name="Mass calculations" sheetId="27" r:id="rId11"/>
+    <sheet name="!!Observables" sheetId="10" r:id="rId12"/>
+    <sheet name="!!Functions" sheetId="11" r:id="rId13"/>
+    <sheet name="!!Reactions" sheetId="12" r:id="rId14"/>
+    <sheet name="!!Rate laws" sheetId="13" r:id="rId15"/>
+    <sheet name="!!dFBA objectives" sheetId="14" r:id="rId16"/>
+    <sheet name="!!dFBA objective reactions" sheetId="15" r:id="rId17"/>
+    <sheet name="!!dFBA objective species" sheetId="16" r:id="rId18"/>
+    <sheet name="!!Parameters" sheetId="17" r:id="rId19"/>
+    <sheet name="!!Stop conditions" sheetId="18" r:id="rId20"/>
+    <sheet name="!!Observations" sheetId="19" r:id="rId21"/>
+    <sheet name="!!Observation sets" sheetId="20" r:id="rId22"/>
+    <sheet name="!!Conclusions" sheetId="21" r:id="rId23"/>
+    <sheet name="!!References" sheetId="22" r:id="rId24"/>
+    <sheet name="!!Authors" sheetId="23" r:id="rId25"/>
+    <sheet name="!!Changes" sheetId="24" r:id="rId26"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId25"/>
-    <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
     <externalReference r:id="rId28"/>
     <externalReference r:id="rId29"/>
+    <externalReference r:id="rId30"/>
+    <externalReference r:id="rId31"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$1:$C$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'!!Compartments'!$A$2:$G$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'!!Parameters'!$A$1:$F$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'!!Reactions'!$A$2:$D$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'!!References'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'!!Parameters'!$A$1:$F$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'!!Reactions'!$A$2:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'!!References'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!!Species types'!$A$2:$K$9</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="18">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="13">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="23">[4]References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="18">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="13">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="23">[4]References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -76,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="309">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
   </si>
@@ -922,6 +924,87 @@
   </si>
   <si>
     <t>!Intention type</t>
+  </si>
+  <si>
+    <t>whole_cell</t>
+  </si>
+  <si>
+    <t>!Component</t>
+  </si>
+  <si>
+    <t>!Attribute</t>
+  </si>
+  <si>
+    <t>!Expected initial value</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>accounted mass</t>
+  </si>
+  <si>
+    <t>accounted volume</t>
+  </si>
+  <si>
+    <t>!Comment</t>
+  </si>
+  <si>
+    <t>Computation for expected initial value</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Data' Id='ExpectedInitialValue' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>initial compartment density * initial compartment volume</t>
+  </si>
+  <si>
+    <t>initial compartment volume</t>
+  </si>
+  <si>
+    <t>accounted mass / initial compartment density</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>compartment</t>
+  </si>
+  <si>
+    <t>mass (g)</t>
+  </si>
+  <si>
+    <t>vol (l)</t>
+  </si>
+  <si>
+    <t>mw (g/mol)</t>
+  </si>
+  <si>
+    <t>initial mean conc (M)</t>
+  </si>
+  <si>
+    <t>c Total</t>
+  </si>
+  <si>
+    <t>e Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>See 'Mass calculations' worksheet</t>
+  </si>
+  <si>
+    <t>sum over s in species in c {conc(s) * mw(st(s)) * vol(comp(s))}</t>
+  </si>
+  <si>
+    <t>Since the cell has only one compartment, same as c</t>
   </si>
 </sst>
 </file>
@@ -933,7 +1016,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -983,6 +1066,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1004,7 +1100,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1060,12 +1156,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF4B084"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF4B084"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF4B084"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF4B084"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF4B084"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF4B084"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFF4B084"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1208,6 +1336,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1231,9 +1365,31 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1573,8 +1729,9 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1843,6 +2000,509 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="47" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>291</v>
+      </c>
+      <c r="F2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3">
+        <v>4.5800000000000003E-15</v>
+      </c>
+      <c r="E3" s="60">
+        <f>'!!Parameters'!D12 * '!!Compartments'!I4</f>
+        <v>4.5800000000000003E-15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C4">
+        <v>4.58E-17</v>
+      </c>
+      <c r="E4" s="60">
+        <f>'!!Compartments'!I4</f>
+        <v>4.58E-17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" s="60">
+        <v>8.2546256000000004E-16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>306</v>
+      </c>
+      <c r="E5">
+        <f>'Mass calculations'!F9</f>
+        <v>8.2546256000000004E-16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6">
+        <v>8.2546256000000003E-18</v>
+      </c>
+      <c r="E6" t="e">
+        <f>E5/#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7">
+        <v>4.5800000000000003E-15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8">
+        <v>4.58E-17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>282</v>
+      </c>
+      <c r="B9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="60">
+        <v>8.2546256000000004E-16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>308</v>
+      </c>
+      <c r="K9" s="64"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10">
+        <v>8.2546256000000003E-18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>308</v>
+      </c>
+      <c r="K10" s="64"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="1">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="65" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="66" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" s="66" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>'!!Species'!A5</f>
+        <v>species_2[c]</v>
+      </c>
+      <c r="B2">
+        <f>'!!Species types'!G$5</f>
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>'!!Initial species concentration'!E5</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2">
+        <v>4.58E-17</v>
+      </c>
+      <c r="F2">
+        <f>B2*C2*E2</f>
+        <v>4.5799999999999998E-20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>'!!Species'!A6</f>
+        <v>species_4[c]</v>
+      </c>
+      <c r="B3">
+        <f>'!!Species types'!G7</f>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>'!!Initial species concentration'!E6</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3">
+        <v>4.58E-17</v>
+      </c>
+      <c r="F3">
+        <f>B3*C3*E3</f>
+        <v>9.1599999999999996E-20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>'!!Species'!A7</f>
+        <v>species_5[c]</v>
+      </c>
+      <c r="B4">
+        <f>'!!Species types'!G8</f>
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f>'!!Initial species concentration'!E7</f>
+        <v>1E-3</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4">
+        <v>4.58E-17</v>
+      </c>
+      <c r="F4">
+        <f>B4*C4*E4</f>
+        <v>2.2899999999999999E-19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>'!!Species'!A8</f>
+        <v>species_6[c]</v>
+      </c>
+      <c r="B5">
+        <f>'!!Species types'!G9</f>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>'!!Initial species concentration'!E8</f>
+        <v>2E-3</v>
+      </c>
+      <c r="D5" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5">
+        <v>4.58E-17</v>
+      </c>
+      <c r="F5">
+        <f>B5*C5*E5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>'!!Species'!A10</f>
+        <v>H2O[c]</v>
+      </c>
+      <c r="B6">
+        <f>'!!Species types'!G$10</f>
+        <v>18.0152</v>
+      </c>
+      <c r="C6">
+        <f>'!!Initial species concentration'!E10</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="64">
+        <v>4.58E-17</v>
+      </c>
+      <c r="F6">
+        <f>B6*C6*E6</f>
+        <v>8.2509616000000004E-16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>'!!Species'!A11</f>
+        <v>species_1[c]</v>
+      </c>
+      <c r="B7">
+        <f>'!!Species types'!G12</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>'!!Initial species concentration'!E11</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="64">
+        <v>4.58E-17</v>
+      </c>
+      <c r="F7">
+        <f>B7*C7*E7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>'!!Species'!A12</f>
+        <v>species_3[c]</v>
+      </c>
+      <c r="B8">
+        <f>'!!Species types'!G13</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>'!!Initial species concentration'!E12</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="64">
+        <v>4.58E-17</v>
+      </c>
+      <c r="F8">
+        <f>B8*C8*E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="67" t="s">
+        <v>303</v>
+      </c>
+      <c r="E9" s="64"/>
+      <c r="F9">
+        <f>SUBTOTAL(9,F2:F8)</f>
+        <v>8.2546256000000004E-16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>'!!Species'!A3</f>
+        <v>species_1[e]</v>
+      </c>
+      <c r="B10">
+        <f>'!!Species types'!G$4</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>'!!Initial species concentration'!E3</f>
+        <v>1.4799999999999999E-4</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10">
+        <f>B10*C10*E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>'!!Species'!A4</f>
+        <v>species_2[e]</v>
+      </c>
+      <c r="B11">
+        <f>'!!Species types'!G$5</f>
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <f>'!!Initial species concentration'!E4</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11">
+        <f>B11*C11*E11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>'!!Species'!A9</f>
+        <v>H2O[e]</v>
+      </c>
+      <c r="B12">
+        <f>'!!Species types'!G$10</f>
+        <v>18.0152</v>
+      </c>
+      <c r="C12">
+        <f>'!!Initial species concentration'!E9</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12">
+        <f>B12*C12*E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="67" t="s">
+        <v>304</v>
+      </c>
+      <c r="F13">
+        <f>SUBTOTAL(9,F10:F12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D14" s="67" t="s">
+        <v>305</v>
+      </c>
+      <c r="F14">
+        <f>SUBTOTAL(9,F2:F12)</f>
+        <v>8.2546256000000004E-16</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:F11">
+    <sortCondition ref="D2:D11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1851,6 +2511,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1899,7 +2560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -1909,6 +2570,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1981,7 +2643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM7"/>
   <sheetViews>
@@ -1991,6 +2653,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2017,11 +2680,11 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -4199,7 +4862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -4209,6 +4872,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4360,7 +5024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -4370,6 +5034,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4448,7 +5113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -4458,6 +5123,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4533,7 +5199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -4543,6 +5209,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4666,7 +5333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
@@ -4674,8 +5341,9 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4887,7 +5555,126 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8:XFD10"/>
+    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="F2" sqref="F2:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1025" width="8.83203125" style="20" customWidth="1"/>
+    <col min="1026" max="1027" width="9" style="20" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="https://github.com/org/repo"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -4897,6 +5684,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4962,7 +5750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W3"/>
   <sheetViews>
@@ -4972,6 +5760,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="Q1" sqref="Q1:T1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4985,26 +5774,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="58" t="s">
         <v>235</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="56" t="s">
+      <c r="H2" s="56"/>
+      <c r="I2" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="Q2" s="57" t="s">
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="Q2" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="56"/>
+      <c r="S2" s="59" t="s">
         <v>238</v>
       </c>
-      <c r="T2" s="54"/>
+      <c r="T2" s="56"/>
     </row>
     <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5088,121 +5877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1025" width="8.83203125" style="20" customWidth="1"/>
-    <col min="1026" max="1027" width="9" style="20" customWidth="1"/>
-    <col min="1028" max="16384" width="9" style="20"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://github.com/org/repo"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -5212,6 +5887,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5263,7 +5939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
@@ -5273,6 +5949,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5288,10 +5965,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="59" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="54"/>
+      <c r="H2" s="56"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5382,7 +6059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -5392,6 +6069,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5469,7 +6147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -5479,6 +6157,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5534,7 +6213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -5544,6 +6223,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5616,11 +6296,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5630,12 +6313,12 @@
     <col min="1028" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -5643,7 +6326,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>31</v>
       </c>
@@ -5651,20 +6334,22 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
@@ -5672,7 +6357,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>54</v>
       </c>
@@ -5685,11 +6370,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B5" sqref="A5:XFD6"/>
+    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5701,12 +6389,12 @@
     <col min="1022" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -5714,12 +6402,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>57</v>
       </c>
@@ -5727,25 +6415,26 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>54</v>
       </c>
@@ -5757,13 +6446,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A3:A4"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5831,6 +6523,10 @@
       <c r="C4" s="20" t="s">
         <v>69</v>
       </c>
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5846,7 +6542,10 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+    </sheetView>
+    <sheetView topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="Q3" sqref="Q3:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5856,7 +6555,7 @@
     <col min="3" max="3" width="23" style="20" customWidth="1"/>
     <col min="4" max="4" width="20" style="20" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="8.83203125" style="20" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="20" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="20" customWidth="1"/>
     <col min="8" max="8" width="16.5" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5" style="12" customWidth="1"/>
@@ -5882,19 +6581,19 @@
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
       <c r="L2" s="37"/>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
@@ -6928,7 +7627,7 @@
       <c r="E3" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="61" t="s">
         <v>76</v>
       </c>
       <c r="G3" s="38" t="s">
@@ -8004,7 +8703,7 @@
       <c r="E4" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="62" t="s">
         <v>88</v>
       </c>
       <c r="G4" s="26" t="s">
@@ -8057,7 +8756,7 @@
       <c r="E5" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="42"/>
+      <c r="F5"/>
       <c r="G5" s="42" t="s">
         <v>89</v>
       </c>
@@ -8108,11 +8807,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8137,14 +8839,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -8197,6 +8899,7 @@
       <c r="B4" s="20" t="s">
         <v>109</v>
       </c>
+      <c r="F4" s="11"/>
       <c r="G4" s="20">
         <v>1</v>
       </c>
@@ -8215,7 +8918,7 @@
       <c r="B5" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5"/>
       <c r="G5" s="20">
         <v>2</v>
       </c>
@@ -8333,11 +9036,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="F3" sqref="F3:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8412,6 +9118,7 @@
       <c r="E4" s="20" t="s">
         <v>128</v>
       </c>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
@@ -8426,6 +9133,7 @@
       <c r="E5" s="20" t="s">
         <v>128</v>
       </c>
+      <c r="F5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
@@ -8540,10 +9248,13 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8666,7 +9377,7 @@
       <c r="E5" s="27">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5"/>
       <c r="G5" s="47" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
fix a computation, & names of density
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-22360" yWindow="10460" windowWidth="22360" windowHeight="11140" tabRatio="993" firstSheet="5" activeTab="6"/>
-    <workbookView xWindow="0" yWindow="9560" windowWidth="33180" windowHeight="12040" tabRatio="500" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="-22360" yWindow="10460" windowWidth="22360" windowHeight="11140" tabRatio="993" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="9560" windowWidth="33180" windowHeight="12040" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
     <definedName name="_FilterDatabase_0_0" localSheetId="23">[4]References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -962,15 +962,9 @@
     <t>Algorithm</t>
   </si>
   <si>
-    <t>initial compartment density * initial compartment volume</t>
-  </si>
-  <si>
     <t>initial compartment volume</t>
   </si>
   <si>
-    <t>accounted mass / initial compartment density</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
@@ -1005,6 +999,12 @@
   </si>
   <si>
     <t>Since the cell has only one compartment, same as c</t>
+  </si>
+  <si>
+    <t>density compartment c * initial compartment volume</t>
+  </si>
+  <si>
+    <t>accounted mass / density compartment c</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1071,6 @@
       <sz val="11"/>
       <color theme="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -1342,6 +1341,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1364,24 +1381,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2006,7 +2005,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2050,7 +2049,7 @@
       <c r="D2" t="s">
         <v>290</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="54" t="s">
         <v>291</v>
       </c>
       <c r="F2" t="s">
@@ -2067,12 +2066,12 @@
       <c r="C3">
         <v>4.5800000000000003E-15</v>
       </c>
-      <c r="E3" s="60">
+      <c r="E3" s="51">
         <f>'!!Parameters'!D12 * '!!Compartments'!I4</f>
         <v>4.5800000000000003E-15</v>
       </c>
       <c r="F3" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2085,12 +2084,12 @@
       <c r="C4">
         <v>4.58E-17</v>
       </c>
-      <c r="E4" s="60">
+      <c r="E4" s="51">
         <f>'!!Compartments'!I4</f>
         <v>4.58E-17</v>
       </c>
       <c r="F4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2100,18 +2099,18 @@
       <c r="B5" t="s">
         <v>288</v>
       </c>
-      <c r="C5" s="60">
+      <c r="C5" s="51">
         <v>8.2546256000000004E-16</v>
       </c>
       <c r="D5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E5">
         <f>'Mass calculations'!F9</f>
         <v>8.2546256000000004E-16</v>
       </c>
       <c r="F5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2124,12 +2123,12 @@
       <c r="C6">
         <v>8.2546256000000003E-18</v>
       </c>
-      <c r="E6" t="e">
-        <f>E5/#REF!</f>
-        <v>#REF!</v>
+      <c r="E6">
+        <f>E5/'!!Parameters'!D12</f>
+        <v>8.2546256000000003E-18</v>
       </c>
       <c r="F6" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2143,7 +2142,7 @@
         <v>4.5800000000000003E-15</v>
       </c>
       <c r="D7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2157,7 +2156,7 @@
         <v>4.58E-17</v>
       </c>
       <c r="D8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2167,13 +2166,13 @@
       <c r="B9" t="s">
         <v>288</v>
       </c>
-      <c r="C9" s="60">
+      <c r="C9" s="51">
         <v>8.2546256000000004E-16</v>
       </c>
       <c r="D9" t="s">
-        <v>308</v>
-      </c>
-      <c r="K9" s="64"/>
+        <v>306</v>
+      </c>
+      <c r="K9" s="55"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2186,9 +2185,9 @@
         <v>8.2546256000000003E-18</v>
       </c>
       <c r="D10" t="s">
-        <v>308</v>
-      </c>
-      <c r="K10" s="64"/>
+        <v>306</v>
+      </c>
+      <c r="K10" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2209,29 +2208,29 @@
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="65" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="56" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="57" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>298</v>
+      </c>
+      <c r="F1" s="57" t="s">
         <v>297</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>301</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>302</v>
-      </c>
-      <c r="D1" s="67" t="s">
-        <v>298</v>
-      </c>
-      <c r="E1" s="66" t="s">
-        <v>300</v>
-      </c>
-      <c r="F1" s="66" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -2247,14 +2246,14 @@
         <f>'!!Initial species concentration'!E5</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="56" t="s">
         <v>83</v>
       </c>
       <c r="E2">
         <v>4.58E-17</v>
       </c>
       <c r="F2">
-        <f>B2*C2*E2</f>
+        <f t="shared" ref="F2:F8" si="0">B2*C2*E2</f>
         <v>4.5799999999999998E-20</v>
       </c>
     </row>
@@ -2271,14 +2270,14 @@
         <f>'!!Initial species concentration'!E6</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="56" t="s">
         <v>83</v>
       </c>
       <c r="E3">
         <v>4.58E-17</v>
       </c>
       <c r="F3">
-        <f>B3*C3*E3</f>
+        <f t="shared" si="0"/>
         <v>9.1599999999999996E-20</v>
       </c>
     </row>
@@ -2295,14 +2294,14 @@
         <f>'!!Initial species concentration'!E7</f>
         <v>1E-3</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="56" t="s">
         <v>83</v>
       </c>
       <c r="E4">
         <v>4.58E-17</v>
       </c>
       <c r="F4">
-        <f>B4*C4*E4</f>
+        <f t="shared" si="0"/>
         <v>2.2899999999999999E-19</v>
       </c>
     </row>
@@ -2319,14 +2318,14 @@
         <f>'!!Initial species concentration'!E8</f>
         <v>2E-3</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="56" t="s">
         <v>83</v>
       </c>
       <c r="E5">
         <v>4.58E-17</v>
       </c>
       <c r="F5">
-        <f>B5*C5*E5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2343,14 +2342,14 @@
         <f>'!!Initial species concentration'!E10</f>
         <v>1</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="55">
         <v>4.58E-17</v>
       </c>
       <c r="F6">
-        <f>B6*C6*E6</f>
+        <f t="shared" si="0"/>
         <v>8.2509616000000004E-16</v>
       </c>
     </row>
@@ -2367,14 +2366,14 @@
         <f>'!!Initial species concentration'!E11</f>
         <v>0</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="64">
+      <c r="E7" s="55">
         <v>4.58E-17</v>
       </c>
       <c r="F7">
-        <f>B7*C7*E7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2391,22 +2390,22 @@
         <f>'!!Initial species concentration'!E12</f>
         <v>0</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="64">
+      <c r="E8" s="55">
         <v>4.58E-17</v>
       </c>
       <c r="F8">
-        <f>B8*C8*E8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="67" t="s">
-        <v>303</v>
-      </c>
-      <c r="E9" s="64"/>
+      <c r="D9" s="58" t="s">
+        <v>301</v>
+      </c>
+      <c r="E9" s="55"/>
       <c r="F9">
         <f>SUBTOTAL(9,F2:F8)</f>
         <v>8.2546256000000004E-16</v>
@@ -2425,7 +2424,7 @@
         <f>'!!Initial species concentration'!E3</f>
         <v>1.4799999999999999E-4</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="56" t="s">
         <v>88</v>
       </c>
       <c r="F10">
@@ -2446,7 +2445,7 @@
         <f>'!!Initial species concentration'!E4</f>
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="56" t="s">
         <v>88</v>
       </c>
       <c r="F11">
@@ -2467,7 +2466,7 @@
         <f>'!!Initial species concentration'!E9</f>
         <v>1</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="56" t="s">
         <v>88</v>
       </c>
       <c r="F12">
@@ -2476,8 +2475,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="67" t="s">
-        <v>304</v>
+      <c r="D13" s="58" t="s">
+        <v>302</v>
       </c>
       <c r="F13">
         <f>SUBTOTAL(9,F10:F12)</f>
@@ -2485,8 +2484,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D14" s="67" t="s">
-        <v>305</v>
+      <c r="D14" s="58" t="s">
+        <v>303</v>
       </c>
       <c r="F14">
         <f>SUBTOTAL(9,F2:F12)</f>
@@ -2680,11 +2679,11 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="65" t="s">
         <v>157</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -5774,26 +5773,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="66" t="s">
         <v>235</v>
       </c>
-      <c r="H2" s="56"/>
-      <c r="I2" s="58" t="s">
+      <c r="H2" s="64"/>
+      <c r="I2" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="Q2" s="59" t="s">
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="Q2" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="R2" s="56"/>
-      <c r="S2" s="59" t="s">
+      <c r="R2" s="64"/>
+      <c r="S2" s="67" t="s">
         <v>238</v>
       </c>
-      <c r="T2" s="56"/>
+      <c r="T2" s="64"/>
     </row>
     <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5965,10 +5964,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="67" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="56"/>
+      <c r="H2" s="64"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -6475,7 +6474,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -6501,7 +6500,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>64</v>
       </c>
@@ -6513,7 +6512,7 @@
       </c>
       <c r="D3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="42" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>67</v>
       </c>
@@ -6581,19 +6580,19 @@
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="61"/>
       <c r="L2" s="37"/>
-      <c r="M2" s="54" t="s">
+      <c r="M2" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
@@ -7627,7 +7626,7 @@
       <c r="E3" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="52" t="s">
         <v>76</v>
       </c>
       <c r="G3" s="38" t="s">
@@ -8703,7 +8702,7 @@
       <c r="E4" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="53" t="s">
         <v>88</v>
       </c>
       <c r="G4" s="26" t="s">
@@ -8808,10 +8807,10 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="F3" sqref="F3"/>
@@ -8839,14 +8838,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">

</xml_diff>

<commit_message>
use FALSE and TRUE instead of 0 and 1 for !Reversible
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\karrlab\wc_sim\tests\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31575" yWindow="8955" windowWidth="30480" windowHeight="9495" tabRatio="993" firstSheet="10" activeTab="17"/>
-    <workbookView xWindow="-30165" yWindow="975" windowWidth="26220" windowHeight="7545" tabRatio="500" firstSheet="12" activeTab="15"/>
+    <workbookView xWindow="-30160" yWindow="980" windowWidth="26220" windowHeight="7540" tabRatio="500" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -66,7 +65,6 @@
     <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -1014,7 +1012,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
@@ -1730,30 +1728,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="15.7109375" style="16" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" style="16" customWidth="1"/>
     <col min="4" max="6" width="9" style="16" hidden="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="16" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
@@ -1764,7 +1758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
@@ -1773,7 +1767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
@@ -1782,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
@@ -1791,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>8</v>
       </c>
@@ -1800,7 +1794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>9</v>
       </c>
@@ -1809,7 +1803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>10</v>
       </c>
@@ -1818,7 +1812,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>11</v>
       </c>
@@ -1827,7 +1821,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
@@ -1836,7 +1830,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>13</v>
       </c>
@@ -1845,7 +1839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>14</v>
       </c>
@@ -1854,7 +1848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>15</v>
       </c>
@@ -1863,7 +1857,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>16</v>
       </c>
@@ -1872,7 +1866,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -1881,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>18</v>
       </c>
@@ -1890,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>19</v>
       </c>
@@ -1899,7 +1893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>20</v>
       </c>
@@ -1908,7 +1902,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>21</v>
       </c>
@@ -1917,7 +1911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>22</v>
       </c>
@@ -1926,7 +1920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>23</v>
       </c>
@@ -1935,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>24</v>
       </c>
@@ -1944,7 +1938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>25</v>
       </c>
@@ -1953,7 +1947,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>26</v>
       </c>
@@ -1962,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>27</v>
       </c>
@@ -2005,24 +1999,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="44" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="44" customWidth="1"/>
     <col min="2" max="2" width="15" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" style="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="44" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="44" customWidth="1"/>
     <col min="6" max="6" width="47" style="44" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="44" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="44" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" style="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>149</v>
       </c>
@@ -2038,7 +2029,7 @@
       <c r="K1" s="49"/>
       <c r="L1" s="49"/>
     </row>
-    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -2058,7 +2049,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
         <v>83</v>
       </c>
@@ -2076,7 +2067,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>83</v>
       </c>
@@ -2094,7 +2085,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
         <v>83</v>
       </c>
@@ -2115,7 +2106,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
         <v>83</v>
       </c>
@@ -2133,7 +2124,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -2147,7 +2138,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2161,7 +2152,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -2175,7 +2166,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>165</v>
       </c>
@@ -2198,20 +2189,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="1"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>167</v>
       </c>
@@ -2231,7 +2221,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'!!Species'!A5</f>
         <v>species_2[c]</v>
@@ -2255,7 +2245,7 @@
         <v>4.5799999999999998E-20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'!!Species'!A6</f>
         <v>species_4[c]</v>
@@ -2279,7 +2269,7 @@
         <v>9.1599999999999996E-20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>'!!Species'!A7</f>
         <v>species_5[c]</v>
@@ -2303,7 +2293,7 @@
         <v>2.2899999999999999E-19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>'!!Species'!A8</f>
         <v>species_6[c]</v>
@@ -2327,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'!!Species'!A10</f>
         <v>H2O[c]</v>
@@ -2351,7 +2341,7 @@
         <v>8.2509616000000004E-16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'!!Species'!A11</f>
         <v>species_1[c]</v>
@@ -2375,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>'!!Species'!A12</f>
         <v>species_3[c]</v>
@@ -2399,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="D9" s="47" t="s">
         <v>173</v>
       </c>
@@ -2408,7 +2398,7 @@
         <v>8.2546256000000004E-16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>'!!Species'!A3</f>
         <v>species_1[e]</v>
@@ -2429,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>'!!Species'!A4</f>
         <v>species_2[e]</v>
@@ -2450,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>'!!Species'!A9</f>
         <v>H2O[e]</v>
@@ -2471,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="D13" s="47" t="s">
         <v>174</v>
       </c>
@@ -2480,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D14" s="47" t="s">
         <v>175</v>
       </c>
@@ -2498,27 +2488,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1026" width="8.85546875" style="49" customWidth="1"/>
+    <col min="1" max="1026" width="8.83203125" style="49" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="49" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -2557,27 +2541,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1026" width="8.85546875" style="49" customWidth="1"/>
+    <col min="1" max="1026" width="8.83203125" style="49" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="49" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -2606,7 +2584,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>179</v>
       </c>
@@ -2618,7 +2596,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>181</v>
       </c>
@@ -2640,28 +2618,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" style="49" customWidth="1"/>
     <col min="2" max="2" width="19" style="49" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="49" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="49" customWidth="1"/>
-    <col min="6" max="10" width="8.85546875" style="49" customWidth="1"/>
-    <col min="11" max="1027" width="8.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="50.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="49" customWidth="1"/>
+    <col min="6" max="10" width="8.83203125" style="49" customWidth="1"/>
+    <col min="11" max="1027" width="8.83203125" style="1" customWidth="1"/>
     <col min="1028" max="1030" width="9" style="1" customWidth="1"/>
     <col min="1031" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1027" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:1027" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1027" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3692,7 +3671,7 @@
       <c r="AML2" s="8"/>
       <c r="AMM2" s="8"/>
     </row>
-    <row r="3" spans="1:1027" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1027" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>29</v>
       </c>
@@ -4749,7 +4728,7 @@
       <c r="AML3" s="8"/>
       <c r="AMM3" s="8"/>
     </row>
-    <row r="4" spans="1:1027" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>191</v>
       </c>
@@ -4762,7 +4741,7 @@
       <c r="D4" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="18" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="49" t="s">
@@ -4779,7 +4758,7 @@
       </c>
       <c r="J4" s="56"/>
     </row>
-    <row r="5" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
         <v>196</v>
       </c>
@@ -4792,7 +4771,7 @@
       <c r="D5" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="18" t="b">
         <v>1</v>
       </c>
       <c r="F5" s="49" t="s">
@@ -4800,7 +4779,7 @@
       </c>
       <c r="J5" s="56"/>
     </row>
-    <row r="6" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
         <v>199</v>
       </c>
@@ -4813,14 +4792,14 @@
       <c r="D6" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="18" t="b">
         <v>1</v>
       </c>
       <c r="F6" s="49" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
         <v>202</v>
       </c>
@@ -4833,7 +4812,7 @@
       <c r="D7" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="18" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="49" t="s">
@@ -4845,6 +4824,11 @@
   <mergeCells count="1">
     <mergeCell ref="G2:I2"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value_x000a__x000a_Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value_x000a__x000a_Select &quot;True&quot; or &quot;False&quot;." sqref="E4:E7">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -4854,34 +4838,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23.7109375" style="49" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="49" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="49" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="49" customWidth="1"/>
-    <col min="6" max="6" width="62.7109375" style="49" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="49" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" style="49" customWidth="1"/>
-    <col min="11" max="1026" width="8.85546875" style="49" customWidth="1"/>
+    <col min="1" max="2" width="23.6640625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="49" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="49" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="62.6640625" style="49" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="49" customWidth="1"/>
+    <col min="8" max="10" width="9.1640625" style="49" customWidth="1"/>
+    <col min="11" max="1026" width="8.83203125" style="49" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="49" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -4919,7 +4897,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
         <v>208</v>
       </c>
@@ -4936,7 +4914,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>211</v>
       </c>
@@ -4953,7 +4931,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
         <v>213</v>
       </c>
@@ -4970,7 +4948,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
         <v>215</v>
       </c>
@@ -4988,7 +4966,7 @@
       </c>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
         <v>218</v>
       </c>
@@ -5016,39 +4994,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="49" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="49" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="49" customWidth="1"/>
     <col min="3" max="3" width="11" style="49" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="49" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="49" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="49" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="49" customWidth="1"/>
     <col min="7" max="7" width="16" style="49" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="49" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="59" t="s">
         <v>29</v>
       </c>
@@ -5086,7 +5058,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
         <v>223</v>
       </c>
@@ -5116,38 +5088,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="5" customWidth="1"/>
     <col min="3" max="3" width="11" style="5" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="14" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="49" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="49" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="49" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" style="49" customWidth="1"/>
-    <col min="11" max="1026" width="8.85546875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="49" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="49" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="49" customWidth="1"/>
+    <col min="9" max="10" width="11.5" style="49" customWidth="1"/>
+    <col min="11" max="1026" width="8.83203125" style="49" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="49" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="59" t="s">
         <v>29</v>
       </c>
@@ -5179,7 +5145,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="58" t="s">
         <v>224</v>
       </c>
@@ -5213,33 +5179,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43" style="5" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="5" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="5" customWidth="1"/>
-    <col min="8" max="1026" width="8.85546875" style="49" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="5" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="5" customWidth="1"/>
+    <col min="8" max="1026" width="8.83203125" style="49" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="49" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
@@ -5274,7 +5234,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>231</v>
       </c>
@@ -5297,7 +5257,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>234</v>
       </c>
@@ -5317,7 +5277,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>236</v>
       </c>
@@ -5347,35 +5307,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="49" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="49" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="49" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="49" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="49" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="49" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="49" customWidth="1"/>
-    <col min="8" max="9" width="9.42578125" style="49" customWidth="1"/>
-    <col min="10" max="1026" width="8.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="49" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="49" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="49" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="49" customWidth="1"/>
+    <col min="8" max="9" width="9.5" style="49" customWidth="1"/>
+    <col min="10" max="1026" width="8.83203125" style="1" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="1" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -5410,7 +5364,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
         <v>240</v>
       </c>
@@ -5427,7 +5381,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>243</v>
       </c>
@@ -5441,7 +5395,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
         <v>245</v>
       </c>
@@ -5455,7 +5409,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
         <v>248</v>
       </c>
@@ -5469,7 +5423,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
         <v>249</v>
       </c>
@@ -5483,7 +5437,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="49" t="s">
         <v>250</v>
       </c>
@@ -5497,7 +5451,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
         <v>251</v>
       </c>
@@ -5511,7 +5465,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="49" t="s">
         <v>252</v>
       </c>
@@ -5525,7 +5479,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="49" t="s">
         <v>254</v>
       </c>
@@ -5536,7 +5490,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="49" t="s">
         <v>92</v>
       </c>
@@ -5547,7 +5501,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49" t="s">
         <v>97</v>
       </c>
@@ -5569,25 +5523,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8:XFD10"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.85546875" style="49" customWidth="1"/>
+    <col min="1" max="1025" width="8.83203125" style="49" customWidth="1"/>
     <col min="1026" max="1028" width="9" style="49" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -5595,7 +5545,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>31</v>
       </c>
@@ -5603,7 +5553,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>33</v>
       </c>
@@ -5611,7 +5561,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>35</v>
       </c>
@@ -5619,7 +5569,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>37</v>
       </c>
@@ -5627,7 +5577,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>39</v>
       </c>
@@ -5635,7 +5585,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>41</v>
       </c>
@@ -5643,7 +5593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>42</v>
       </c>
@@ -5651,22 +5601,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>47</v>
       </c>
@@ -5684,30 +5634,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="49" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="49" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="49" customWidth="1"/>
     <col min="4" max="4" width="16" style="49" customWidth="1"/>
-    <col min="5" max="1026" width="8.85546875" style="49" customWidth="1"/>
+    <col min="5" max="1026" width="8.83203125" style="49" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="49" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -5736,7 +5680,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
         <v>258</v>
       </c>
@@ -5761,20 +5705,19 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="9" style="49" customWidth="1"/>
     <col min="4" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="67" t="s">
         <v>262</v>
       </c>
@@ -5796,7 +5739,7 @@
       </c>
       <c r="T2" s="65"/>
     </row>
-    <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -5882,28 +5825,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="49" customWidth="1"/>
-    <col min="2" max="3" width="13.28515625" style="49" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="49" customWidth="1"/>
-    <col min="7" max="1017" width="9.140625" customWidth="1"/>
+    <col min="2" max="3" width="13.33203125" style="49" customWidth="1"/>
+    <col min="4" max="6" width="9.1640625" style="49" customWidth="1"/>
+    <col min="7" max="1017" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -5923,13 +5860,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -5945,28 +5882,27 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="49" customWidth="1"/>
-    <col min="3" max="14" width="9.140625" style="49" customWidth="1"/>
-    <col min="15" max="1024" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="49" customWidth="1"/>
+    <col min="3" max="14" width="9.1640625" style="49" customWidth="1"/>
+    <col min="15" max="1024" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="68" t="s">
         <v>276</v>
       </c>
       <c r="H2" s="65"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -6010,35 +5946,35 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
@@ -6059,28 +5995,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="17" width="8.85546875" style="49" customWidth="1"/>
-    <col min="18" max="1025" width="8.85546875" style="1" customWidth="1"/>
+    <col min="1" max="17" width="8.83203125" style="49" customWidth="1"/>
+    <col min="18" max="1025" width="8.83203125" style="1" customWidth="1"/>
     <col min="1026" max="1028" width="9" style="1" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -6147,26 +6077,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="9" style="49" customWidth="1"/>
     <col min="4" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -6213,26 +6137,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="9" style="49" customWidth="1"/>
     <col min="4" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -6294,25 +6212,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.85546875" style="49" customWidth="1"/>
+    <col min="1" max="1025" width="8.83203125" style="49" customWidth="1"/>
     <col min="1026" max="1028" width="9" style="49" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -6320,7 +6234,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>31</v>
       </c>
@@ -6328,7 +6242,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>51</v>
       </c>
@@ -6336,12 +6250,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
@@ -6349,7 +6263,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>54</v>
       </c>
@@ -6364,27 +6278,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B5" sqref="A5:XFD6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="49" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="49" customWidth="1"/>
-    <col min="3" max="1019" width="8.85546875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="49" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="49" customWidth="1"/>
+    <col min="3" max="1019" width="8.83203125" style="15" customWidth="1"/>
     <col min="1020" max="1022" width="9" style="15" customWidth="1"/>
     <col min="1023" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -6392,12 +6302,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>57</v>
       </c>
@@ -6405,7 +6315,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>58</v>
       </c>
@@ -6413,17 +6323,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>54</v>
       </c>
@@ -6437,32 +6347,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="49" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="49" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="49" customWidth="1"/>
     <col min="3" max="3" width="27" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.85546875" style="49" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="1026" width="8.85546875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="8.83203125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="1026" width="8.83203125" style="1" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="1" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -6488,7 +6392,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
         <v>64</v>
       </c>
@@ -6500,7 +6404,7 @@
       </c>
       <c r="D3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>67</v>
       </c>
@@ -6521,40 +6425,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMR9"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="49" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="49" customWidth="1"/>
     <col min="2" max="2" width="12" style="49" customWidth="1"/>
     <col min="3" max="3" width="23" style="49" customWidth="1"/>
     <col min="4" max="4" width="20" style="49" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" style="49" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="49" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="12" customWidth="1"/>
-    <col min="13" max="19" width="8.85546875" style="12" customWidth="1"/>
-    <col min="20" max="20" width="34.42578125" style="12" customWidth="1"/>
-    <col min="21" max="1035" width="8.85546875" style="12" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" style="49" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="49" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="12" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="12" customWidth="1"/>
+    <col min="13" max="19" width="8.83203125" style="12" customWidth="1"/>
+    <col min="20" max="20" width="34.5" style="12" customWidth="1"/>
+    <col min="21" max="1035" width="8.83203125" style="12" customWidth="1"/>
     <col min="1036" max="1038" width="9" style="12" customWidth="1"/>
     <col min="1039" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1032" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1032" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:1032" s="48" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1032" s="48" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -7592,7 +7490,7 @@
       <c r="AMQ2" s="8"/>
       <c r="AMR2" s="8"/>
     </row>
-    <row r="3" spans="1:1032" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1032" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>29</v>
       </c>
@@ -8668,7 +8566,7 @@
       <c r="AMQ3" s="28"/>
       <c r="AMR3" s="28"/>
     </row>
-    <row r="4" spans="1:1032" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1032" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="49" t="s">
         <v>83</v>
       </c>
@@ -8721,7 +8619,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:1032" s="30" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1032" s="30" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>88</v>
       </c>
@@ -8771,7 +8669,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:1032" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:1032" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <autoFilter ref="A2:G4"/>
   <mergeCells count="2">
@@ -8787,36 +8685,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="49" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="49" customWidth="1"/>
-    <col min="3" max="5" width="8.85546875" style="49" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="49" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="8.85546875" style="49" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="1028" width="8.85546875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="49" customWidth="1"/>
+    <col min="3" max="5" width="8.83203125" style="49" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="49" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.83203125" style="49" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="14" max="1028" width="8.83203125" style="49" customWidth="1"/>
     <col min="1029" max="1031" width="9" style="49" customWidth="1"/>
     <col min="1032" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="63" t="s">
         <v>100</v>
       </c>
@@ -8826,7 +8718,7 @@
       <c r="G2" s="65"/>
       <c r="H2" s="65"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>29</v>
       </c>
@@ -8870,7 +8762,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>108</v>
       </c>
@@ -8889,7 +8781,7 @@
       </c>
       <c r="J4" s="51"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
         <v>111</v>
       </c>
@@ -8907,7 +8799,7 @@
       </c>
       <c r="J5" s="51"/>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
         <v>113</v>
       </c>
@@ -8926,7 +8818,7 @@
       </c>
       <c r="J6" s="51"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
         <v>115</v>
       </c>
@@ -8945,7 +8837,7 @@
       </c>
       <c r="J7" s="51"/>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="49" t="s">
         <v>117</v>
       </c>
@@ -8964,7 +8856,7 @@
       </c>
       <c r="J8" s="51"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
         <v>119</v>
       </c>
@@ -8982,7 +8874,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="49" t="s">
         <v>122</v>
       </c>
@@ -9013,28 +8905,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="15.42578125" style="49" customWidth="1"/>
-    <col min="7" max="1026" width="9.140625" style="49" customWidth="1"/>
+    <col min="1" max="6" width="15.5" style="49" customWidth="1"/>
+    <col min="7" max="1026" width="9.1640625" style="49" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="49" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>29</v>
       </c>
@@ -9066,7 +8952,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
         <v>127</v>
       </c>
@@ -9080,7 +8966,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>129</v>
       </c>
@@ -9094,7 +8980,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
         <v>130</v>
       </c>
@@ -9108,7 +8994,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
         <v>131</v>
       </c>
@@ -9122,7 +9008,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
         <v>132</v>
       </c>
@@ -9136,7 +9022,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="49" t="s">
         <v>133</v>
       </c>
@@ -9150,7 +9036,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
         <v>134</v>
       </c>
@@ -9164,7 +9050,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="49" t="s">
         <v>135</v>
       </c>
@@ -9178,7 +9064,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="49" t="s">
         <v>136</v>
       </c>
@@ -9192,7 +9078,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="49" t="s">
         <v>137</v>
       </c>
@@ -9220,30 +9106,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="49" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="49" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="50" customWidth="1"/>
-    <col min="8" max="12" width="8.85546875" style="49" customWidth="1"/>
-    <col min="13" max="1026" width="8.85546875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="49" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="49" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="52" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="49" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="50" customWidth="1"/>
+    <col min="8" max="12" width="8.83203125" style="49" customWidth="1"/>
+    <col min="13" max="1026" width="8.83203125" style="10" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="10" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>138</v>
       </c>
@@ -9254,7 +9134,7 @@
       <c r="F1" s="22"/>
       <c r="G1" s="23"/>
     </row>
-    <row r="2" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>29</v>
       </c>
@@ -9292,7 +9172,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>140</v>
       </c>
@@ -9313,7 +9193,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>142</v>
       </c>
@@ -9334,7 +9214,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>143</v>
       </c>
@@ -9352,7 +9232,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>144</v>
       </c>
@@ -9371,7 +9251,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>145</v>
       </c>
@@ -9390,7 +9270,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>146</v>
       </c>
@@ -9409,7 +9289,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>147</v>
       </c>
@@ -9428,7 +9308,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
remove flux bounds from reaction_1, which isn't modeled by dfba
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30160" yWindow="980" windowWidth="26220" windowHeight="7540" tabRatio="500" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="25600" windowHeight="11560" tabRatio="500" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="309">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -662,9 +662,6 @@
   </si>
   <si>
     <t>s^-1</t>
-  </si>
-  <si>
-    <t>M s^-1</t>
   </si>
   <si>
     <t>reaction_2</t>
@@ -2618,8 +2615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4747,29 +4744,20 @@
       <c r="F4" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="G4" s="49">
-        <v>0</v>
-      </c>
-      <c r="H4" s="49">
-        <v>1</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>195</v>
-      </c>
       <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>196</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>197</v>
       </c>
       <c r="C5" s="49" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" s="18" t="b">
         <v>1</v>
@@ -4781,16 +4769,16 @@
     </row>
     <row r="6" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>199</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>200</v>
       </c>
       <c r="C6" s="49" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E6" s="18" t="b">
         <v>1</v>
@@ -4801,16 +4789,16 @@
     </row>
     <row r="7" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="49" t="s">
         <v>202</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>203</v>
       </c>
       <c r="C7" s="49" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E7" s="18" t="b">
         <v>0</v>
@@ -4856,7 +4844,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4867,10 +4855,10 @@
         <v>31</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>206</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>207</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>107</v>
@@ -4899,16 +4887,16 @@
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>191</v>
       </c>
       <c r="D3" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="49" t="s">
         <v>209</v>
-      </c>
-      <c r="F3" s="49" t="s">
-        <v>210</v>
       </c>
       <c r="G3" s="49" t="s">
         <v>194</v>
@@ -4916,16 +4904,16 @@
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" s="49" t="s">
         <v>211</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="F4" s="49" t="s">
-        <v>212</v>
       </c>
       <c r="G4" s="49" t="s">
         <v>194</v>
@@ -4933,16 +4921,16 @@
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="49" t="s">
         <v>213</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>199</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="F5" s="49" t="s">
-        <v>214</v>
       </c>
       <c r="G5" s="49" t="s">
         <v>194</v>
@@ -4950,16 +4938,16 @@
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="49" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="49" t="s">
-        <v>199</v>
-      </c>
-      <c r="D6" s="49" t="s">
+      <c r="F6" s="49" t="s">
         <v>216</v>
-      </c>
-      <c r="F6" s="49" t="s">
-        <v>217</v>
       </c>
       <c r="G6" s="49" t="s">
         <v>194</v>
@@ -4968,16 +4956,16 @@
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="F7" s="49" t="s">
         <v>218</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>202</v>
-      </c>
-      <c r="D7" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="F7" s="49" t="s">
-        <v>219</v>
       </c>
       <c r="G7" s="49" t="s">
         <v>194</v>
@@ -5017,7 +5005,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -5037,10 +5025,10 @@
         <v>81</v>
       </c>
       <c r="F2" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="59" t="s">
         <v>221</v>
-      </c>
-      <c r="G2" s="59" t="s">
-        <v>222</v>
       </c>
       <c r="H2" s="59" t="s">
         <v>44</v>
@@ -5060,14 +5048,14 @@
     </row>
     <row r="3" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" s="57"/>
       <c r="C3" s="57" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3" s="57" t="s">
         <v>93</v>
@@ -5110,7 +5098,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5127,7 +5115,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F2" s="59" t="s">
         <v>44</v>
@@ -5147,10 +5135,10 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C3" s="57" t="s">
         <v>64</v>
@@ -5165,7 +5153,7 @@
       <c r="G3" s="57"/>
       <c r="H3" s="57"/>
       <c r="I3" s="58" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J3" s="57"/>
     </row>
@@ -5196,7 +5184,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5207,7 +5195,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>139</v>
@@ -5236,13 +5224,13 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D3" s="49" t="s">
         <v>136</v>
@@ -5251,21 +5239,21 @@
         <v>-3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>235</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>130</v>
@@ -5274,18 +5262,18 @@
         <v>-4</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>237</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D5" s="49" t="s">
         <v>137</v>
@@ -5294,7 +5282,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -5326,7 +5314,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5343,7 +5331,7 @@
         <v>101</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>81</v>
@@ -5366,10 +5354,10 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>240</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>241</v>
       </c>
       <c r="D3" s="49">
         <v>0.3</v>
@@ -5378,15 +5366,15 @@
         <v>93</v>
       </c>
       <c r="J3" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>243</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>244</v>
       </c>
       <c r="D4" s="49">
         <v>1</v>
@@ -5397,38 +5385,38 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="49" t="s">
         <v>245</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>246</v>
       </c>
       <c r="D5" s="49">
         <v>1</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D6" s="4">
         <v>2000</v>
       </c>
       <c r="F6" s="49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D7" s="4">
         <v>2.9999999999999997E-4</v>
@@ -5439,38 +5427,38 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="49" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D8" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F8" s="49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D9" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F9" s="49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="49" t="s">
         <v>252</v>
-      </c>
-      <c r="C10" s="49" t="s">
-        <v>253</v>
       </c>
       <c r="D10" s="4">
         <v>1E-3</v>
@@ -5481,13 +5469,13 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11" s="4">
         <v>6.02214075862E+23</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5498,7 +5486,7 @@
         <v>100</v>
       </c>
       <c r="F12" s="49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5509,7 +5497,7 @@
         <v>1000</v>
       </c>
       <c r="F13" s="49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -5648,7 +5636,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5682,16 +5670,16 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="49" t="s">
         <v>258</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>259</v>
       </c>
       <c r="D3" s="49" t="s">
         <v>93</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -5714,16 +5702,16 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="67" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H2" s="65"/>
       <c r="I2" s="67" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J2" s="65"/>
       <c r="K2" s="65"/>
@@ -5731,11 +5719,11 @@
       <c r="M2" s="65"/>
       <c r="N2" s="65"/>
       <c r="Q2" s="68" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R2" s="65"/>
       <c r="S2" s="68" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="T2" s="65"/>
     </row>
@@ -5750,7 +5738,7 @@
         <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>81</v>
@@ -5759,10 +5747,10 @@
         <v>107</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>57</v>
@@ -5774,19 +5762,19 @@
         <v>72</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>31</v>
@@ -5837,7 +5825,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5848,7 +5836,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>44</v>
@@ -5893,12 +5881,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="68" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H2" s="65"/>
     </row>
@@ -5913,7 +5901,7 @@
         <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>81</v>
@@ -5940,10 +5928,10 @@
         <v>54</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6007,7 +5995,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6018,46 +6006,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>282</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>283</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>107</v>
       </c>
       <c r="H2" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>291</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>292</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>44</v>
@@ -6087,7 +6075,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6098,28 +6086,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>299</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>300</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>44</v>
@@ -6147,7 +6135,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6161,25 +6149,25 @@
         <v>107</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>307</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>308</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>44</v>
@@ -6197,10 +6185,10 @@
         <v>54</v>
       </c>
       <c r="P2" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q2" s="13" t="s">
         <v>277</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -8905,7 +8893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
fix tests in test_multialgorithm_simulation.py
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1500" windowWidth="25600" windowHeight="11560" tabRatio="500" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="4000" yWindow="620" windowWidth="19920" windowHeight="6480" tabRatio="500" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -1405,9 +1405,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Compartments"/>
+      <sheetName val="#REF"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1418,9 +1420,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Parameters"/>
+      <sheetName val="#REF"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1431,9 +1435,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Reactions"/>
+      <sheetName val="#REF"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1444,9 +1450,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="References"/>
+      <sheetName val="#REF"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4826,11 +4834,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23.6640625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="49" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="49" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="49" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" style="49" customWidth="1"/>

</xml_diff>

<commit_message>
create and use a transformation that sets all standard deviations of data in a whole-cell model used by a simulation to 0
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="620" windowWidth="19920" windowHeight="6480" tabRatio="500" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="-47480" yWindow="22540" windowWidth="19420" windowHeight="14920" tabRatio="500" firstSheet="12" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
     <definedName name="_FilterDatabase_0_0" localSheetId="23">[4]References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="311">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -1004,6 +1004,12 @@
   </si>
   <si>
     <t>mole / gDCW</t>
+  </si>
+  <si>
+    <t>Extra param for testing SetStdDevsToZero transformation</t>
+  </si>
+  <si>
+    <t>extra_param</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1194,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1357,6 +1363,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2623,7 +2632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -2652,11 +2661,11 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="67" t="s">
         <v>184</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -5304,9 +5313,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5509,6 +5520,23 @@
       </c>
       <c r="F13" s="49" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="49" t="s">
+        <v>310</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>309</v>
+      </c>
+      <c r="D14" s="60">
+        <v>1</v>
+      </c>
+      <c r="E14" s="60">
+        <v>1</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -5717,26 +5745,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="68" t="s">
         <v>261</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="67" t="s">
+      <c r="H2" s="66"/>
+      <c r="I2" s="68" t="s">
         <v>262</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="Q2" s="68" t="s">
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="Q2" s="69" t="s">
         <v>263</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="68" t="s">
+      <c r="R2" s="66"/>
+      <c r="S2" s="69" t="s">
         <v>264</v>
       </c>
-      <c r="T2" s="65"/>
+      <c r="T2" s="66"/>
     </row>
     <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5896,10 +5924,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="H2" s="65"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -6459,19 +6487,19 @@
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
       <c r="L2" s="31"/>
-      <c r="M2" s="63" t="s">
+      <c r="M2" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
@@ -8708,14 +8736,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">

</xml_diff>